<commit_message>
add orderNum zone,zone template
</commit_message>
<xml_diff>
--- a/server/zone-template/Zone_Template.xlsx
+++ b/server/zone-template/Zone_Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuongh\AppData\Roaming\Skype\My Skype Received Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\wi-backend\server\zone-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F80BACE9-0E0D-4F35-8D34-2BEC66E82BCC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="zone_template" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="194">
   <si>
     <t>id</t>
   </si>
@@ -604,12 +603,15 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>order_num</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1053,11 +1055,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1068,9 +1070,10 @@
     <col min="4" max="4" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1089,8 +1092,11 @@
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G1" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickBot="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1109,11 +1115,14 @@
       <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5" thickBot="1">
+    <row r="3" spans="1:8" ht="16.5" thickBot="1">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1132,8 +1141,11 @@
       <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" thickBot="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1152,8 +1164,11 @@
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" thickBot="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1172,8 +1187,11 @@
       <c r="F5" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" thickBot="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1192,8 +1210,11 @@
       <c r="F6" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" thickBot="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1212,8 +1233,11 @@
       <c r="F7" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" thickBot="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1232,8 +1256,11 @@
       <c r="F8" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" thickBot="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1252,8 +1279,11 @@
       <c r="F9" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" thickBot="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1272,8 +1302,11 @@
       <c r="F10" s="7" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" thickBot="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1292,8 +1325,11 @@
       <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" thickBot="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1312,8 +1348,11 @@
       <c r="F12" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" thickBot="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1332,8 +1371,11 @@
       <c r="F13" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" thickBot="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1352,8 +1394,11 @@
       <c r="F14" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" thickBot="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1372,8 +1417,11 @@
       <c r="F15" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16.5" thickBot="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1392,8 +1440,11 @@
       <c r="F16" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" thickBot="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1412,8 +1463,11 @@
       <c r="F17" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" thickBot="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1432,8 +1486,11 @@
       <c r="F18" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" thickBot="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1452,8 +1509,11 @@
       <c r="F19" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1472,8 +1532,11 @@
       <c r="F20" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16.5" thickBot="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1492,8 +1555,11 @@
       <c r="F21" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16.5" thickBot="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1512,8 +1578,11 @@
       <c r="F22" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G22" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1532,8 +1601,11 @@
       <c r="F23" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.5" thickBot="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1552,8 +1624,11 @@
       <c r="F24" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G24" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="16.5" thickBot="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1572,8 +1647,11 @@
       <c r="F25" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G25" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16.5" thickBot="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1592,8 +1670,11 @@
       <c r="F26" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G26" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="16.5" thickBot="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1612,8 +1693,11 @@
       <c r="F27" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G27" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="16.5" thickBot="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1632,8 +1716,11 @@
       <c r="F28" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G28" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="16.5" thickBot="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1652,8 +1739,11 @@
       <c r="F29" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G29" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16.5" thickBot="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1672,8 +1762,11 @@
       <c r="F30" s="7" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" s="1" customFormat="1" ht="16.5" thickBot="1">
+      <c r="G30" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="16.5" thickBot="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1692,8 +1785,11 @@
       <c r="F31" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="16.5" thickBot="1">
+      <c r="G31" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1712,8 +1808,11 @@
       <c r="F32" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G32" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="16.5" thickBot="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1732,8 +1831,11 @@
       <c r="F33" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G33" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="16.5" thickBot="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1752,8 +1854,11 @@
       <c r="F34" s="8" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G34" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="16.5" thickBot="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1772,8 +1877,11 @@
       <c r="F35" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G35" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="16.5" thickBot="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1792,8 +1900,11 @@
       <c r="F36" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G36" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="16.5" thickBot="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1812,8 +1923,11 @@
       <c r="F37" s="9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G37" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="16.5" thickBot="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1832,8 +1946,11 @@
       <c r="F38" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G38" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="16.5" thickBot="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1852,8 +1969,11 @@
       <c r="F39" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G39" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="16.5" thickBot="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1872,8 +1992,11 @@
       <c r="F40" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G40" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="16.5" thickBot="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1892,8 +2015,11 @@
       <c r="F41" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G41" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="16.5" thickBot="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1912,8 +2038,11 @@
       <c r="F42" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G42" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="16.5" thickBot="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1932,8 +2061,11 @@
       <c r="F43" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G43" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="16.5" thickBot="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1952,11 +2084,14 @@
       <c r="F44" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G44" s="18" t="s">
+      <c r="G44" s="1">
+        <v>43</v>
+      </c>
+      <c r="H44" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="16.5" thickBot="1">
+    <row r="45" spans="1:8" ht="16.5" thickBot="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1975,8 +2110,11 @@
       <c r="F45" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G45" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="16.5" thickBot="1">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1995,11 +2133,14 @@
       <c r="F46" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="G46" s="1">
+        <v>45</v>
+      </c>
+      <c r="H46" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="16.5" thickBot="1">
+    <row r="47" spans="1:8" ht="16.5" thickBot="1">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2018,8 +2159,11 @@
       <c r="F47" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G47" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="16.5" thickBot="1">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2038,8 +2182,11 @@
       <c r="F48" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G48" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="16.5" thickBot="1">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2058,8 +2205,11 @@
       <c r="F49" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G49" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="16.5" thickBot="1">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2078,8 +2228,11 @@
       <c r="F50" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G50" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="16.5" thickBot="1">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2098,8 +2251,11 @@
       <c r="F51" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G51" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="16.5" thickBot="1">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2118,8 +2274,11 @@
       <c r="F52" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G52" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="16.5" thickBot="1">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2138,8 +2297,11 @@
       <c r="F53" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G53" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="16.5" thickBot="1">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2158,11 +2320,14 @@
       <c r="F54" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G54" s="18" t="s">
+      <c r="G54" s="1">
+        <v>53</v>
+      </c>
+      <c r="H54" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="16.5" thickBot="1">
+    <row r="55" spans="1:8" ht="16.5" thickBot="1">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2181,8 +2346,11 @@
       <c r="F55" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G55" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="16.5" thickBot="1">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2201,11 +2369,14 @@
       <c r="F56" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G56" s="18" t="s">
+      <c r="G56" s="1">
+        <v>55</v>
+      </c>
+      <c r="H56" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15.75" thickBot="1">
+    <row r="57" spans="1:8" ht="15.75" thickBot="1">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2224,8 +2395,11 @@
       <c r="F57" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" thickBot="1">
+      <c r="G57" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" thickBot="1">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2244,8 +2418,11 @@
       <c r="F58" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G58" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="16.5" thickBot="1">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2264,8 +2441,11 @@
       <c r="F59" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G59" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="16.5" thickBot="1">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2284,8 +2464,11 @@
       <c r="F60" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" thickBot="1">
+      <c r="G60" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickBot="1">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2304,8 +2487,11 @@
       <c r="F61" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G61" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="16.5" thickBot="1">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2324,8 +2510,11 @@
       <c r="F62" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G62" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="16.5" thickBot="1">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2344,8 +2533,11 @@
       <c r="F63" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G63" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="16.5" thickBot="1">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2364,8 +2556,11 @@
       <c r="F64" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G64" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="16.5" thickBot="1">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2384,8 +2579,11 @@
       <c r="F65" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G65" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="16.5" thickBot="1">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2404,8 +2602,11 @@
       <c r="F66" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G66" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="16.5" thickBot="1">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2424,8 +2625,11 @@
       <c r="F67" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G67" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="16.5" thickBot="1">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2444,8 +2648,11 @@
       <c r="F68" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G68" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="16.5" thickBot="1">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2464,8 +2671,11 @@
       <c r="F69" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G69" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="16.5" thickBot="1">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2484,8 +2694,11 @@
       <c r="F70" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G70" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="16.5" thickBot="1">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2504,8 +2717,11 @@
       <c r="F71" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G71" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="16.5" thickBot="1">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2524,8 +2740,11 @@
       <c r="F72" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G72" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="16.5" thickBot="1">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2544,11 +2763,14 @@
       <c r="F73" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G73" s="18" t="s">
+      <c r="G73" s="1">
+        <v>72</v>
+      </c>
+      <c r="H73" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="16.5" thickBot="1">
+    <row r="74" spans="1:8" ht="16.5" thickBot="1">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -2567,8 +2789,11 @@
       <c r="F74" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G74" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="16.5" thickBot="1">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -2587,8 +2812,11 @@
       <c r="F75" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G75" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="16.5" thickBot="1">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -2607,11 +2835,14 @@
       <c r="F76" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G76" s="18" t="s">
+      <c r="G76" s="1">
+        <v>75</v>
+      </c>
+      <c r="H76" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="16.5" thickBot="1">
+    <row r="77" spans="1:8" ht="16.5" thickBot="1">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -2630,8 +2861,11 @@
       <c r="F77" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G77" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="16.5" thickBot="1">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -2650,8 +2884,11 @@
       <c r="F78" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G78" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="16.5" thickBot="1">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -2670,8 +2907,11 @@
       <c r="F79" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G79" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="16.5" thickBot="1">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -2690,8 +2930,11 @@
       <c r="F80" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G80" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="16.5" thickBot="1">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -2710,8 +2953,11 @@
       <c r="F81" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G81" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="16.5" thickBot="1">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -2730,8 +2976,11 @@
       <c r="F82" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G82" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="16.5" thickBot="1">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -2750,8 +2999,11 @@
       <c r="F83" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G83" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="16.5" thickBot="1">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -2770,8 +3022,11 @@
       <c r="F84" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G84" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="16.5" thickBot="1">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -2790,8 +3045,11 @@
       <c r="F85" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G85" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="16.5" thickBot="1">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -2810,8 +3068,11 @@
       <c r="F86" s="11" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G86" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="16.5" thickBot="1">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -2830,11 +3091,14 @@
       <c r="F87" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="G87" s="18" t="s">
+      <c r="G87" s="1">
+        <v>86</v>
+      </c>
+      <c r="H87" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="16.5" thickBot="1">
+    <row r="88" spans="1:8" ht="16.5" thickBot="1">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -2853,8 +3117,11 @@
       <c r="F88" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G88" s="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="16.5" thickBot="1">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -2873,8 +3140,11 @@
       <c r="F89" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="16.5" thickBot="1">
+      <c r="G89" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="16.5" thickBot="1">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -2893,8 +3163,11 @@
       <c r="F90" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="15.75" thickBot="1">
+      <c r="G90" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" thickBot="1">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -2913,24 +3186,27 @@
       <c r="F91" s="4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="15.75" thickBot="1">
+      <c r="G91" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15.75" thickBot="1">
       <c r="C92" s="4"/>
       <c r="F92" s="4"/>
     </row>
-    <row r="93" spans="1:7" ht="16.5" thickBot="1">
+    <row r="93" spans="1:8" ht="16.5" thickBot="1">
       <c r="C93" s="11"/>
       <c r="F93" s="4"/>
     </row>
-    <row r="94" spans="1:7" ht="16.5" thickBot="1">
+    <row r="94" spans="1:8" ht="16.5" thickBot="1">
       <c r="C94" s="11"/>
       <c r="F94" s="4"/>
     </row>
-    <row r="95" spans="1:7" ht="16.5" thickBot="1">
+    <row r="95" spans="1:8" ht="16.5" thickBot="1">
       <c r="C95" s="11"/>
       <c r="F95" s="4"/>
     </row>
-    <row r="96" spans="1:7" ht="16.5" thickBot="1">
+    <row r="96" spans="1:8" ht="16.5" thickBot="1">
       <c r="C96" s="11"/>
       <c r="F96" s="4"/>
     </row>

</xml_diff>